<commit_message>
Se tiene ahora el lag de 20 dias, con retorno, se aplanan las fechas para que no queden datos en blanco.
</commit_message>
<xml_diff>
--- a/Data/1_preprocess/DIAGNOSTICO_CATEGORIAS.xlsx
+++ b/Data/1_preprocess/DIAGNOSTICO_CATEGORIAS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="122">
   <si>
     <t>Columna</t>
   </si>
@@ -127,51 +127,6 @@
     <t>PRICE_Nickel_Futures_commodities</t>
   </si>
   <si>
-    <t>PRICE_US_Cotton_#2_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_Lumber_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Cocoa_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Coffee_C_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_Orange_Juice_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Sugar_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Corn_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Wheat_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_Oats_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_Rough_Rice_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Soybean_Meal_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Soybean_Oil_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_US_Soybeans_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_Feeder_Cattle_Futures_commodities</t>
-  </si>
-  <si>
-    <t>PRICE_Live_Cattle_Futures_commodities</t>
-  </si>
-  <si>
     <t>PRICE_Iron_ore_fines_62%_Fe_CFR_Futures_commodities</t>
   </si>
   <si>
@@ -199,6 +154,15 @@
     <t>PRICE_PHP_ZAR_exchange_rate</t>
   </si>
   <si>
+    <t>PRICE_USDCOP-US_Dollar_Colombian_Peso_exchange_rate</t>
+  </si>
+  <si>
+    <t>PRICE_Colombia_5_Year_Bond_bond</t>
+  </si>
+  <si>
+    <t>PRICE_Colombia_10_Year_Bond_bond</t>
+  </si>
+  <si>
     <t>ESI_GACDISA_US_Empire_State_Index_business_confidence</t>
   </si>
   <si>
@@ -271,6 +235,12 @@
     <t>Actual_Eurozone_Unemployment_Rate_unemployment_rate</t>
   </si>
   <si>
+    <t>Actual_IPC Colombia_economics</t>
+  </si>
+  <si>
+    <t>Actual_IPC EEUU_economics</t>
+  </si>
+  <si>
     <t>DGS10_US_10Y_Treasury_bond</t>
   </si>
   <si>
@@ -371,6 +341,9 @@
   </si>
   <si>
     <t>ICSA_US_Initial_Jobless_Claims_unemployment_rate</t>
+  </si>
+  <si>
+    <t>DGS10_DGS10_bond</t>
   </si>
   <si>
     <t>Sin categoría</t>
@@ -764,7 +737,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -783,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -791,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -799,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -807,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -815,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -823,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -831,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -839,7 +812,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -847,7 +820,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -855,7 +828,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -863,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -871,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -879,7 +852,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -887,7 +860,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -895,7 +868,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -903,7 +876,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -911,7 +884,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -919,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -927,7 +900,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -935,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -943,7 +916,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -951,7 +924,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -959,7 +932,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -967,7 +940,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -975,7 +948,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -983,7 +956,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -991,7 +964,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -999,7 +972,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1007,7 +980,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1015,7 +988,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1023,7 +996,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1031,7 +1004,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1039,7 +1012,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1047,7 +1020,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1055,7 +1028,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1063,7 +1036,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1071,7 +1044,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1079,7 +1052,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1087,7 +1060,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1095,7 +1068,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1103,7 +1076,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1111,7 +1084,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1119,7 +1092,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1127,7 +1100,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1135,7 +1108,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1143,7 +1116,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1151,7 +1124,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1159,7 +1132,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1167,7 +1140,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1175,7 +1148,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1183,7 +1156,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1191,7 +1164,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1199,7 +1172,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1207,7 +1180,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1215,7 +1188,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1223,7 +1196,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1231,7 +1204,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1239,7 +1212,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1247,7 +1220,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1255,7 +1228,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1263,7 +1236,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1271,7 +1244,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1279,7 +1252,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1287,7 +1260,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1295,7 +1268,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1303,7 +1276,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1311,7 +1284,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1319,7 +1292,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1327,7 +1300,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1335,7 +1308,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1343,7 +1316,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1351,7 +1324,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1359,7 +1332,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1367,7 +1340,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1375,7 +1348,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1383,7 +1356,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1391,7 +1364,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1399,7 +1372,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1407,7 +1380,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1415,7 +1388,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1423,7 +1396,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1431,7 +1404,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1439,7 +1412,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1447,7 +1420,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1455,7 +1428,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1463,7 +1436,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1471,7 +1444,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1479,7 +1452,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1487,7 +1460,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1495,7 +1468,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1503,7 +1476,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1511,7 +1484,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1519,7 +1492,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1527,7 +1500,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1535,7 +1508,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1543,7 +1516,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1551,7 +1524,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1559,7 +1532,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1567,7 +1540,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1575,7 +1548,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1583,7 +1556,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1591,7 +1564,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1599,7 +1572,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1607,7 +1580,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1615,7 +1588,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1623,7 +1596,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1631,7 +1604,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1639,79 +1612,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" t="s">
-        <v>110</v>
-      </c>
-      <c r="B110" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
         <v>111</v>
-      </c>
-      <c r="B111" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" t="s">
-        <v>112</v>
-      </c>
-      <c r="B112" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" t="s">
-        <v>113</v>
-      </c>
-      <c r="B113" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" t="s">
-        <v>114</v>
-      </c>
-      <c r="B114" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" t="s">
-        <v>115</v>
-      </c>
-      <c r="B115" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" t="s">
-        <v>116</v>
-      </c>
-      <c r="B116" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" t="s">
-        <v>117</v>
-      </c>
-      <c r="B117" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" t="s">
-        <v>118</v>
-      </c>
-      <c r="B118" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>